<commit_message>
time table entry added
</commit_message>
<xml_diff>
--- a/Dokumente/Zeitschaetzung.xlsx
+++ b/Dokumente/Zeitschaetzung.xlsx
@@ -543,19 +543,19 @@
     </xf>
   </cellXfs>
   <cellStyles count="13">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -892,10 +892,10 @@
   <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
@@ -1314,7 +1314,9 @@
       <c r="F30" s="28">
         <v>2</v>
       </c>
-      <c r="G30" s="9"/>
+      <c r="G30" s="9">
+        <v>2</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -1327,7 +1329,9 @@
       <c r="F31" s="29">
         <v>1</v>
       </c>
-      <c r="G31" s="3"/>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
@@ -1340,7 +1344,9 @@
       <c r="F32" s="29">
         <v>1</v>
       </c>
-      <c r="G32" s="3"/>
+      <c r="G32" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
@@ -1353,7 +1359,9 @@
       <c r="F33" s="29">
         <v>1</v>
       </c>
-      <c r="G33" s="3"/>
+      <c r="G33" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
@@ -1366,7 +1374,9 @@
       <c r="F34" s="29">
         <v>1</v>
       </c>
-      <c r="G34" s="3"/>
+      <c r="G34" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E35" s="16"/>
@@ -1464,7 +1474,6 @@
         <v>11</v>
       </c>
       <c r="B43" s="2">
-        <f>F36</f>
         <v>0</v>
       </c>
       <c r="C43" s="2">

</xml_diff>